<commit_message>
PSP 박영우 UPDATE 11.12
</commit_message>
<xml_diff>
--- a/관리산출물PMP:PSP/PSP/박영우/신수동크러셔_psp_20151154_박영우.xlsx
+++ b/관리산출물PMP:PSP/PSP/박영우/신수동크러셔_psp_20151154_박영우.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywooo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66010190-5EE7-4D57-9A55-CE1F85E754CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E19ACB-86CF-4627-AEE3-72A2892BB712}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>PSP: Personal Software Process</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>작성자명:</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>Start</t>
@@ -103,6 +100,14 @@
   </si>
   <si>
     <t>SAD 스켈레톤 코드 작성 및 선행개발</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERD 설계 및 산출물 작성</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity Class 설계 및 산출물 작성</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -471,7 +476,7 @@
   <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -485,7 +490,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -515,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -528,23 +533,21 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -565,10 +568,10 @@
         <v>45</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -589,16 +592,16 @@
         <v>45.000000000000028</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="9">
         <f>SUM(E6:E123)</f>
-        <v>645.00000000000034</v>
+        <v>785.00000000000034</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="12">
         <v>0.79166666666666663</v>
@@ -614,7 +617,7 @@
         <v>70.000000000000028</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -635,7 +638,7 @@
         <v>25.000000000000071</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -656,7 +659,7 @@
         <v>30.000000000000053</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -677,7 +680,7 @@
         <v>30.000000000000053</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -698,12 +701,12 @@
         <v>40.000000000000142</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
-        <v>43733</v>
+        <v>43763</v>
       </c>
       <c r="B13" s="12">
         <v>0.625</v>
@@ -715,64 +718,100 @@
         <v>0</v>
       </c>
       <c r="E13" s="14">
-        <f t="shared" ref="E13:E14" si="2">(C13-B13)*1440-D13</f>
+        <f t="shared" ref="E13:E15" si="2">(C13-B13)*1440-D13</f>
         <v>180</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
-        <v>43763</v>
+        <v>43774</v>
       </c>
       <c r="B14" s="12">
-        <v>0.625</v>
+        <v>0.5625</v>
       </c>
       <c r="C14" s="12">
-        <v>0.75</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D14" s="13">
         <v>0</v>
       </c>
       <c r="E14" s="14">
-        <f t="shared" ref="E14:E18" si="3">(C14-B14)*1440-D14</f>
-        <v>180</v>
+        <f t="shared" si="2"/>
+        <v>59.999999999999943</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>43780</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" ref="E15:E16" si="3">(C15-B15)*1440-D15</f>
+        <v>70.000000000000071</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>43781</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D16" s="13">
+        <v>20</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" ref="E16:E20" si="4">(C16-B16)*1440-D16</f>
+        <v>189.99999999999997</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="7"/>
-    </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="13">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -783,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F19" s="7"/>
@@ -796,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F20" s="7"/>
@@ -1082,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="14">
-        <f t="shared" ref="E42:E73" si="4">(C42-B42)*1440-D42</f>
+        <f t="shared" ref="E42:E73" si="5">(C42-B42)*1440-D42</f>
         <v>0</v>
       </c>
       <c r="F42" s="7"/>
@@ -1095,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F43" s="7"/>
@@ -1108,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F44" s="7"/>
@@ -1121,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F45" s="7"/>
@@ -1134,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F46" s="7"/>
@@ -1147,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F47" s="7"/>
@@ -1160,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F48" s="7"/>
@@ -1173,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F49" s="7"/>
@@ -1186,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F50" s="7"/>
@@ -1199,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F51" s="7"/>
@@ -1212,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F52" s="7"/>
@@ -1225,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F53" s="7"/>
@@ -1238,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F54" s="7"/>
@@ -1251,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F55" s="7"/>
@@ -1264,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F56" s="7"/>
@@ -1277,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F57" s="7"/>
@@ -1290,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F58" s="7"/>
@@ -1303,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F59" s="7"/>
@@ -1316,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F60" s="7"/>
@@ -1329,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="E61" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F61" s="7"/>
@@ -1342,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="E62" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F62" s="7"/>
@@ -1355,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F63" s="7"/>
@@ -1368,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="E64" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F64" s="7"/>
@@ -1381,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F65" s="7"/>
@@ -1394,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F66" s="7"/>
@@ -1407,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="E67" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F67" s="7"/>
@@ -1420,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F68" s="7"/>
@@ -1433,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F69" s="7"/>
@@ -1446,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F70" s="7"/>
@@ -1459,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="E71" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71" s="7"/>
@@ -1472,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="E72" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72" s="7"/>
@@ -1485,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="E73" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73" s="7"/>
@@ -1498,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="14">
-        <f t="shared" ref="E74:E105" si="5">(C74-B74)*1440-D74</f>
+        <f t="shared" ref="E74:E105" si="6">(C74-B74)*1440-D74</f>
         <v>0</v>
       </c>
       <c r="F74" s="7"/>
@@ -1511,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F75" s="7"/>
@@ -1524,7 +1563,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F76" s="7"/>
@@ -1537,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="E77" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F77" s="7"/>
@@ -1550,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="E78" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F78" s="7"/>
@@ -1563,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="E79" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F79" s="7"/>
@@ -1576,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="E80" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F80" s="7"/>
@@ -1589,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F81" s="7"/>
@@ -1602,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="E82" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F82" s="7"/>
@@ -1615,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="E83" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F83" s="7"/>
@@ -1628,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="E84" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F84" s="7"/>
@@ -1641,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F85" s="7"/>
@@ -1654,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F86" s="7"/>
@@ -1667,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="E87" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F87" s="7"/>
@@ -1680,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F88" s="7"/>
@@ -1693,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F89" s="7"/>
@@ -1706,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="E90" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F90" s="7"/>
@@ -1719,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="E91" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F91" s="7"/>
@@ -1732,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="E92" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F92" s="7"/>
@@ -1745,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F93" s="7"/>
@@ -1758,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F94" s="7"/>
@@ -1771,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="E95" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F95" s="7"/>
@@ -1784,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="E96" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F96" s="7"/>
@@ -1797,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="E97" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F97" s="7"/>
@@ -1810,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="E98" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F98" s="7"/>
@@ -1823,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="E99" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F99" s="7"/>
@@ -1836,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="E100" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F100" s="7"/>
@@ -1849,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="E101" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F101" s="7"/>
@@ -1862,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="E102" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F102" s="7"/>
@@ -1875,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="E103" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F103" s="7"/>
@@ -1888,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="E104" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F104" s="7"/>
@@ -1901,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="E105" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F105" s="7"/>
@@ -1914,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="E106" s="14">
-        <f t="shared" ref="E106:E123" si="6">(C106-B106)*1440-D106</f>
+        <f t="shared" ref="E106:E123" si="7">(C106-B106)*1440-D106</f>
         <v>0</v>
       </c>
       <c r="F106" s="7"/>
@@ -1927,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="E107" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F107" s="7"/>
@@ -1940,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="E108" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F108" s="7"/>
@@ -1953,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="E109" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F109" s="7"/>
@@ -1966,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="E110" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F110" s="7"/>
@@ -1979,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="E111" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F111" s="7"/>
@@ -1992,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="E112" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F112" s="7"/>
@@ -2005,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="E113" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F113" s="7"/>
@@ -2018,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="E114" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F114" s="7"/>
@@ -2031,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="E115" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F115" s="7"/>
@@ -2044,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="E116" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F116" s="7"/>
@@ -2057,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="E117" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F117" s="7"/>
@@ -2070,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="E118" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F118" s="7"/>
@@ -2083,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="E119" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F119" s="7"/>
@@ -2096,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="E120" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F120" s="7"/>
@@ -2109,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="E121" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F121" s="7"/>
@@ -2122,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="E122" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F122" s="7"/>
@@ -2135,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="E123" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F123" s="7"/>

</xml_diff>